<commit_message>
added AVP 2023 data
</commit_message>
<xml_diff>
--- a/data/Administracion_de_viviendas_publicas/avpAsignadas2017_23.xlsx
+++ b/data/Administracion_de_viviendas_publicas/avpAsignadas2017_23.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel.santiago\Documents\Aplicacion Indicadores PARE - Copy\data\Administracion_de_viviendas_publicas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix.baez\Documents\ViolenciaGeneroPR\data\Administracion_de_viviendas_publicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3645B9-468E-43B3-BA5F-8D8700E60D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="1095" yWindow="2175" windowWidth="15180" windowHeight="11130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -77,8 +80,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -86,16 +89,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Century"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -103,14 +118,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,11 +454,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -483,7 +512,7 @@
         <v>12</v>
       </c>
       <c r="H2">
-        <v>4</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -509,7 +538,7 @@
         <v>19</v>
       </c>
       <c r="H3">
-        <v>10</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -535,7 +564,7 @@
         <v>13</v>
       </c>
       <c r="H4">
-        <v>6</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -561,7 +590,7 @@
         <v>25</v>
       </c>
       <c r="H5">
-        <v>13</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -587,7 +616,7 @@
         <v>12</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -613,7 +642,7 @@
         <v>6</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -639,7 +668,7 @@
         <v>6</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -665,7 +694,7 @@
         <v>10</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -691,7 +720,7 @@
         <v>25</v>
       </c>
       <c r="H10">
-        <v>14</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -717,10 +746,10 @@
         <v>35</v>
       </c>
       <c r="H11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -743,8 +772,9 @@
       <c r="G12">
         <v>163</v>
       </c>
-      <c r="H12">
-        <v>73</v>
+      <c r="H12" s="2">
+        <f>SUM(H2:H11)</f>
+        <v>215.99999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Administración de Vivienda Pública
</commit_message>
<xml_diff>
--- a/data/Administracion_de_viviendas_publicas/avpAsignadas2017_23.xlsx
+++ b/data/Administracion_de_viviendas_publicas/avpAsignadas2017_23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix.baez\Documents\ViolenciaGeneroPR\data\Administracion_de_viviendas_publicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3645B9-468E-43B3-BA5F-8D8700E60D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0C826F-B176-4A23-9695-53B031FAAE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="2175" windowWidth="15180" windowHeight="11130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14820" yWindow="690" windowWidth="12300" windowHeight="12750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Región </t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>*2023</t>
   </si>
 </sst>
 </file>
@@ -159,9 +156,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -199,7 +196,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -305,7 +302,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -447,7 +444,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -458,7 +455,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -485,8 +482,8 @@
       <c r="G1" s="1">
         <v>2022</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>12</v>
+      <c r="H1" s="1">
+        <v>2023</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -512,7 +509,7 @@
         <v>12</v>
       </c>
       <c r="H2">
-        <v>21.6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -538,7 +535,7 @@
         <v>19</v>
       </c>
       <c r="H3">
-        <v>21.6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -564,7 +561,7 @@
         <v>13</v>
       </c>
       <c r="H4">
-        <v>21.6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -590,7 +587,7 @@
         <v>25</v>
       </c>
       <c r="H5">
-        <v>21.6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -616,7 +613,7 @@
         <v>12</v>
       </c>
       <c r="H6">
-        <v>21.6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -642,7 +639,7 @@
         <v>6</v>
       </c>
       <c r="H7">
-        <v>21.6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -668,7 +665,7 @@
         <v>6</v>
       </c>
       <c r="H8">
-        <v>21.6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -694,7 +691,7 @@
         <v>10</v>
       </c>
       <c r="H9">
-        <v>21.6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -720,7 +717,7 @@
         <v>25</v>
       </c>
       <c r="H10">
-        <v>21.6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -746,7 +743,7 @@
         <v>35</v>
       </c>
       <c r="H11">
-        <v>21.6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -774,7 +771,7 @@
       </c>
       <c r="H12" s="2">
         <f>SUM(H2:H11)</f>
-        <v>215.99999999999997</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>